<commit_message>
new data depot data files (removing box links from excel)
</commit_message>
<xml_diff>
--- a/data/depot/Spending Drivers - Admin - Trust in Government.xlsx
+++ b/data/depot/Spending Drivers - Admin - Trust in Government.xlsx
@@ -635,9 +635,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -665,6 +662,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -970,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,22 +991,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2272,7 +2278,7 @@
       <c r="G47" s="5">
         <v>605</v>
       </c>
-      <c r="J47" s="12">
+      <c r="J47" s="9">
         <f>D47+C47</f>
         <v>72</v>
       </c>
@@ -2441,46 +2447,47 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="15"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="12"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="18"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="15"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="18"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="15"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="21"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A55:G58"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>